<commit_message>
update water stress indicatoren en figures
Water stress indicators were added to the analysis
extra figure showing Y and WPET response was added for publication
purpose
Manual was updated
</commit_message>
<xml_diff>
--- a/Information/variables.xlsx
+++ b/Information/variables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="190">
   <si>
     <t>Yactstats</t>
   </si>
@@ -89,9 +89,6 @@
     <t>TSIDeltastats</t>
   </si>
   <si>
-    <t>Absolute difference ofDSI stats as compared to scenario 1</t>
-  </si>
-  <si>
     <t>Absolute difference of DSI stats as compared to scenario 1</t>
   </si>
   <si>
@@ -149,12 +146,6 @@
     <t>yield of each crop in each cyle(average over different landunits in catchment)</t>
   </si>
   <si>
-    <t>WPET of each crop in each cyle(average over different landunits in catchment)</t>
-  </si>
-  <si>
-    <t>DSI of each crop in each cyle(average over different landunits in catchment)</t>
-  </si>
-  <si>
     <t>TSI of each crop in each cyle(average over different landunits in catchment)</t>
   </si>
   <si>
@@ -552,6 +543,48 @@
   </si>
   <si>
     <t>Growing degree days accumulated on that day in each land unit for each timestep and scenario</t>
+  </si>
+  <si>
+    <t>WSI</t>
+  </si>
+  <si>
+    <t>WSIstats</t>
+  </si>
+  <si>
+    <t>WSIDeltastats</t>
+  </si>
+  <si>
+    <t>BWSI</t>
+  </si>
+  <si>
+    <t>BWSIstats</t>
+  </si>
+  <si>
+    <t>BWSIDeltastats</t>
+  </si>
+  <si>
+    <t>WSI stats for each crop over different cyles</t>
+  </si>
+  <si>
+    <t>Absolute difference of WSI stats as compared to scenario 1</t>
+  </si>
+  <si>
+    <t>BWSI stats for each crop over different cyles</t>
+  </si>
+  <si>
+    <t>Absolute difference of BWSI stats as compared to scenario 1</t>
+  </si>
+  <si>
+    <t>ET Crop water productivity of each crop in each cyle(average over different landunits in catchment)</t>
+  </si>
+  <si>
+    <t>Drought stress index of each crop in each cyle(average over different landunits in catchment)</t>
+  </si>
+  <si>
+    <t>Water stress index of each crop in each cyle(average over different landunits in catchment)</t>
+  </si>
+  <si>
+    <t>Biomass water stress index of each crop in each cyle(average over different landunits in catchment)</t>
   </si>
 </sst>
 </file>
@@ -902,10 +935,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -920,7 +953,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -937,647 +970,647 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
         <v>93</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1587,13 +1620,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1610,7 +1643,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1630,7 +1663,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1639,10 +1672,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1650,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1662,7 +1695,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1670,7 +1703,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1687,10 +1720,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1702,7 +1735,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1710,7 +1743,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -1719,7 +1752,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -1730,7 +1763,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1739,10 +1772,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1750,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -1762,7 +1795,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1770,7 +1803,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1782,15 +1815,15 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
         <v>75</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1810,7 +1843,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1819,10 +1852,10 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1830,7 +1863,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1842,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1850,7 +1883,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1867,10 +1900,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1879,18 +1912,18 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1902,15 +1935,15 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1922,35 +1955,35 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1959,18 +1992,18 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1982,55 +2015,55 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" t="s">
-        <v>41</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2039,58 +2072,58 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>66</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -2099,18 +2132,18 @@
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -2119,38 +2152,38 @@
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -2159,18 +2192,18 @@
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -2179,38 +2212,38 @@
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" t="s">
-        <v>56</v>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -2219,58 +2252,58 @@
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
         <v>61</v>
       </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" t="s">
-        <v>85</v>
+      <c r="F41" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -2279,18 +2312,18 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -2302,7 +2335,127 @@
         <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>89</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>